<commit_message>
2021/06/07 22:58 更改Debug模式为True 修复admin后台答题信息展示bug
</commit_message>
<xml_diff>
--- a/util/SeriusStudents.xlsx
+++ b/util/SeriusStudents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pythoncode\PythonLastTest\util\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74F70D8D-D5EE-410B-BA35-8CC3D9DFD8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFD54951-B553-4F98-8A9B-81FCF6D37B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2340" windowWidth="16200" windowHeight="12645" xr2:uid="{73E78A6D-8516-4369-A174-37F24EB46D8C}"/>
+    <workbookView xWindow="3660" yWindow="2340" windowWidth="16200" windowHeight="12645" xr2:uid="{85CE7051-9CCA-4A82-8542-0BC89BEC536C}"/>
   </bookViews>
   <sheets>
     <sheet name="重度焦虑学生" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>学号</t>
   </si>
@@ -36,61 +36,55 @@
     <t>得分</t>
   </si>
   <si>
-    <t>郭娴瑗</t>
-  </si>
-  <si>
-    <t>吕贵真</t>
+    <t>符群舒</t>
+  </si>
+  <si>
+    <t>孔兴</t>
+  </si>
+  <si>
+    <t>桂云伯</t>
+  </si>
+  <si>
+    <t>苗淑媛</t>
+  </si>
+  <si>
+    <t>黄寒</t>
+  </si>
+  <si>
+    <t>阮德以</t>
   </si>
   <si>
     <t>幸辉</t>
   </si>
   <si>
-    <t>潘媛</t>
-  </si>
-  <si>
-    <t>邴功</t>
-  </si>
-  <si>
-    <t>缪玲</t>
-  </si>
-  <si>
-    <t>吴姣芝</t>
-  </si>
-  <si>
-    <t>乔毅</t>
-  </si>
-  <si>
-    <t>卞霄</t>
+    <t>王妍</t>
+  </si>
+  <si>
+    <t>姜梦</t>
+  </si>
+  <si>
+    <t>牛裕环</t>
+  </si>
+  <si>
+    <t>盛腾鹏</t>
   </si>
   <si>
     <t>黄菁航</t>
   </si>
   <si>
-    <t>苍会</t>
-  </si>
-  <si>
-    <t>华娣秋</t>
-  </si>
-  <si>
-    <t>靳博滢</t>
-  </si>
-  <si>
-    <t>红之</t>
-  </si>
-  <si>
-    <t>瞿伟</t>
-  </si>
-  <si>
-    <t>霍文贞</t>
-  </si>
-  <si>
-    <t>路娥</t>
-  </si>
-  <si>
-    <t>步腾</t>
-  </si>
-  <si>
-    <t>东桂承</t>
+    <t>向悦</t>
+  </si>
+  <si>
+    <t>向天纨</t>
+  </si>
+  <si>
+    <t>桓军伦</t>
+  </si>
+  <si>
+    <t>牧兴</t>
+  </si>
+  <si>
+    <t>阮丹毓</t>
   </si>
 </sst>
 </file>
@@ -453,8 +447,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE517F0B-591B-4972-B905-A6C3B1F5BEA8}">
-  <dimension ref="A1:C20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38AECBA-C068-41B3-BC3F-9B7EAC25F5D6}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -478,106 +472,106 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2201804688</v>
+        <v>2201804568</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>83.75</v>
+        <v>78.75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2201804678</v>
+        <v>2201804800</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2201804914</v>
+        <v>2201804904</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4">
-        <v>78.75</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2201804935</v>
+        <v>2201804856</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5">
-        <v>78.75</v>
+        <v>73.75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2201804810</v>
+        <v>2201804433</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
-        <v>75</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2201804972</v>
+        <v>2201804854</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
-        <v>75</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2201804446</v>
+        <v>2201804914</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>73.75</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2201804859</v>
+        <v>2201804488</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9">
-        <v>73.75</v>
+        <v>71.25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2201804963</v>
+        <v>2201804505</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10">
-        <v>73.75</v>
+        <v>71.25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2201804443</v>
+        <v>2201804804</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -588,7 +582,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2201804774</v>
+        <v>2201804978</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -599,7 +593,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2201804412</v>
+        <v>2201804443</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -610,7 +604,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2201804536</v>
+        <v>2201804465</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -621,7 +615,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2201804549</v>
+        <v>2201804645</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -632,7 +626,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2201804639</v>
+        <v>2201804694</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -643,7 +637,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2201804650</v>
+        <v>2201804727</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -654,34 +648,12 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2201804744</v>
+        <v>2201804921</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>2201804763</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>2201804953</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
         <v>70</v>
       </c>
     </row>

</xml_diff>